<commit_message>
merge corresponding parquet file to csv by id
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,22 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scout\OneDrive\Documents\Python_code\Child_Mind_Institute\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thiennguyenba/Documents/School/DataScience/Child-mind-institute-club/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BFDF206-1D5F-4C41-B5B3-FD29DB826548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5001E1-0780-7E46-9D90-FF5686DA786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="4440" windowWidth="21600" windowHeight="9195" xr2:uid="{F38225D3-037D-4079-BB33-31E10AB1611D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F38225D3-037D-4079-BB33-31E10AB1611D}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={C48B1459-8401-6E4F-B75C-95655DD51C42}</author>
+  </authors>
+  <commentList>
+    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{C48B1459-8401-6E4F-B75C-95655DD51C42}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Deleted because not in test df</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -735,7 +753,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -913,6 +931,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1076,9 +1106,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1135,6 +1167,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Thien Nguyen Ba" id="{E25C849B-CAAE-684B-9BB0-0D301B272637}" userId="e1b127e8d0008194" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1452,48 +1490,56 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B56" dT="2024-10-29T20:19:13.23" personId="{E25C849B-CAAE-684B-9BB0-0D301B272637}" id="{C48B1459-8401-6E4F-B75C-95655DD51C42}">
+    <text>Deleted because not in test df</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79770E63-C3DA-4433-9FD2-CE0A28DB8417}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79770E63-C3DA-4433-9FD2-CE0A28DB8417}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" customWidth="1"/>
     <col min="3" max="3" width="131" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1507,7 +1553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1527,7 +1573,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1541,7 +1587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1561,7 +1607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1584,7 +1630,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1598,7 +1644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1618,7 +1664,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1632,7 +1678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1646,7 +1692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1660,7 +1706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1674,7 +1720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1688,7 +1734,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1702,7 +1748,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1716,7 +1762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1736,7 +1782,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1750,7 +1796,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1764,7 +1810,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1778,7 +1824,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1798,7 +1844,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1812,7 +1858,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1832,7 +1878,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1846,7 +1892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1866,7 +1912,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -1880,7 +1926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1900,7 +1946,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1914,7 +1960,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1934,7 +1980,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1948,7 +1994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1968,7 +2014,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1982,7 +2028,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2002,7 +2048,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -2016,7 +2062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -2036,7 +2082,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -2056,7 +2102,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2076,7 +2122,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -2090,7 +2136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -2104,7 +2150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>85</v>
       </c>
@@ -2118,7 +2164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2132,7 +2178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2146,7 +2192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -2160,7 +2206,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -2174,7 +2220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -2188,7 +2234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2202,7 +2248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2222,7 +2268,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -2236,7 +2282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -2250,7 +2296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -2264,7 +2310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -2278,7 +2324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -2292,7 +2338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -2312,7 +2358,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -2326,7 +2372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>126</v>
       </c>
@@ -2346,7 +2392,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -2360,11 +2406,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>130</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C56" t="s">
@@ -2380,11 +2426,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>130</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>132</v>
       </c>
       <c r="C57" t="s">
@@ -2400,11 +2446,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>130</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
       <c r="C58" t="s">
@@ -2420,11 +2466,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>130</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C59" t="s">
@@ -2440,11 +2486,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>130</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C60" t="s">
@@ -2460,11 +2506,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>130</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C61" t="s">
@@ -2480,11 +2526,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>130</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C62" t="s">
@@ -2500,11 +2546,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>130</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>146</v>
       </c>
       <c r="C63" t="s">
@@ -2520,11 +2566,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>130</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C64" t="s">
@@ -2540,11 +2586,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>130</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>150</v>
       </c>
       <c r="C65" t="s">
@@ -2560,11 +2606,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>130</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>152</v>
       </c>
       <c r="C66" t="s">
@@ -2580,11 +2626,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>130</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>154</v>
       </c>
       <c r="C67" t="s">
@@ -2600,11 +2646,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>130</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C68" t="s">
@@ -2620,11 +2666,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>130</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C69" t="s">
@@ -2640,11 +2686,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>130</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C70" t="s">
@@ -2660,11 +2706,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>130</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C71" t="s">
@@ -2680,11 +2726,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>130</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>164</v>
       </c>
       <c r="C72" t="s">
@@ -2700,11 +2746,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>130</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C73" t="s">
@@ -2720,11 +2766,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>130</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>168</v>
       </c>
       <c r="C74" t="s">
@@ -2740,11 +2786,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>130</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>170</v>
       </c>
       <c r="C75" t="s">
@@ -2760,11 +2806,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>130</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="3" t="s">
         <v>172</v>
       </c>
       <c r="C76" t="s">
@@ -2780,11 +2826,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>130</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>174</v>
       </c>
       <c r="C77" t="s">
@@ -2797,7 +2843,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>177</v>
       </c>
@@ -2817,7 +2863,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>177</v>
       </c>
@@ -2831,7 +2877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -2845,7 +2891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -2865,7 +2911,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>183</v>
       </c>
@@ -2887,5 +2933,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>